<commit_message>
Veel gezeik met dictionaries enzo
</commit_message>
<xml_diff>
--- a/Main/Antwoordenblad_MT1463_1466_V03.xlsx
+++ b/Main/Antwoordenblad_MT1463_1466_V03.xlsx
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>3.922625326993233</v>
+        <v>3.100992589961451</v>
       </c>
     </row>
     <row r="17" ht="35.4" customHeight="1">
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="D37" s="23" t="n">
-        <v>70.88850209079619</v>
+        <v>70.91120726548422</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1">
@@ -1504,7 +1504,7 @@
         </is>
       </c>
       <c r="D38" s="23" t="n">
-        <v>0.0001099427400106407</v>
+        <v>-0.0004327642678354389</v>
       </c>
     </row>
     <row r="39">
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="D39" s="23" t="n">
-        <v>6.282111553326359</v>
+        <v>7.104063194937617</v>
       </c>
     </row>
     <row r="41">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="D49" s="7" t="n">
-        <v>2.980232238769531e-08</v>
+        <v>-2.980232238769531e-08</v>
       </c>
     </row>
     <row r="50">
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>-1106151.284012488</v>
+        <v>-6563531.254794854</v>
       </c>
     </row>
     <row r="51">
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>-26425.66355516203</v>
+        <v>104018.5367347449</v>
       </c>
     </row>
     <row r="52" ht="40.8" customHeight="1">
@@ -1734,7 +1734,7 @@
         </is>
       </c>
       <c r="D57" s="7" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" ht="14.4" customHeight="1">
@@ -1749,7 +1749,7 @@
         </is>
       </c>
       <c r="D58" s="7" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="59" ht="14.4" customHeight="1">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>24.988</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" ht="31.8" customHeight="1">
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="D69" s="7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="D77" s="7" t="n">
-        <v>44.13382562299425</v>
+        <v>44.146</v>
       </c>
     </row>
     <row r="78">
@@ -2038,7 +2038,7 @@
         </is>
       </c>
       <c r="D81" s="23" t="n">
-        <v>15.988</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82">
@@ -2073,7 +2073,7 @@
         </is>
       </c>
       <c r="D84" s="7" t="n">
-        <v>16.125</v>
+        <v>16.13</v>
       </c>
     </row>
     <row r="85" ht="14.4" customHeight="1">
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="D85" s="7" t="n">
-        <v>30.06091281149713</v>
+        <v>30.073</v>
       </c>
     </row>
     <row r="86" ht="14.4" customHeight="1">
@@ -2138,7 +2138,7 @@
         </is>
       </c>
       <c r="D89" s="7" t="n">
-        <v>44.13382562299425</v>
+        <v>44.146</v>
       </c>
     </row>
     <row r="90" ht="36.6" customHeight="1">

</xml_diff>

<commit_message>
Bloed Zweet en Tranen
boys
De sterkte functies staan nu in de sterkte main
De stabiliteitsfuncties in de stabliteits main
De asymptoten, zijn weggewerkt
Mijn ziel, is gestorven, mijn taak, voldaan
</commit_message>
<xml_diff>
--- a/Main/Antwoordenblad_MT1463_1466_V03.xlsx
+++ b/Main/Antwoordenblad_MT1463_1466_V03.xlsx
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="D8" s="10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" ht="28.8" customHeight="1">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="D11" s="22" t="inlineStr">
         <is>
-          <t>46.5347</t>
+          <t>46.5378</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
         </is>
       </c>
       <c r="D12" s="22" t="n">
-        <v>470550.3126380809</v>
+        <v>470659.0411009961</v>
       </c>
     </row>
     <row r="13" ht="35.4" customHeight="1">
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>2.590607086687617</v>
+        <v>2.592784728379922</v>
       </c>
     </row>
     <row r="17" ht="35.4" customHeight="1">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D23" s="7" t="inlineStr">
         <is>
-          <t>23.976</t>
+          <t>23.98</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>14.988</v>
+        <v>14.99</v>
       </c>
     </row>
     <row r="25">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D25" s="7" t="inlineStr">
         <is>
-          <t>7.988</t>
+          <t>7.99</t>
         </is>
       </c>
     </row>
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D36" s="23" t="n">
-        <v>-240358422.507975</v>
+        <v>-240462406.8648</v>
       </c>
     </row>
     <row r="37">
@@ -1489,7 +1489,7 @@
         </is>
       </c>
       <c r="D37" s="23" t="n">
-        <v>70.8839227245594</v>
+        <v>70.882868698804</v>
       </c>
     </row>
     <row r="38" ht="18" customHeight="1">
@@ -1504,7 +1504,7 @@
         </is>
       </c>
       <c r="D38" s="23" t="n">
-        <v>1.79106342960379e-06</v>
+        <v>-7.530965586057507e-07</v>
       </c>
     </row>
     <row r="39">
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="D39" s="23" t="n">
-        <v>7.613924182893339</v>
+        <v>7.613300179624092</v>
       </c>
     </row>
     <row r="41">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="D43" s="7" t="n">
-        <v>240358422.507975</v>
+        <v>240462406.8648</v>
       </c>
     </row>
     <row r="44">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="D44" s="7" t="n">
-        <v>70.8839</v>
+        <v>70.8827</v>
       </c>
     </row>
     <row r="45">
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="D46" s="7" t="n">
-        <v>4.2096</v>
+        <v>4.2107</v>
       </c>
     </row>
     <row r="48" ht="39" customHeight="1">
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="D50" s="7" t="n">
-        <v>-5462.039249679584</v>
+        <v>-40565.72044589418</v>
       </c>
     </row>
     <row r="51">
@@ -1655,7 +1655,7 @@
         </is>
       </c>
       <c r="D51" s="7" t="n">
-        <v>-430.4971805512905</v>
+        <v>181.0914110839367</v>
       </c>
     </row>
     <row r="52" ht="40.8" customHeight="1">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="D59" s="7" t="n">
-        <v>24.988</v>
+        <v>24.99</v>
       </c>
     </row>
     <row r="60" ht="31.8" customHeight="1">
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="D77" s="7" t="n">
-        <v>44.13382562299425</v>
+        <v>44.13582562299425</v>
       </c>
     </row>
     <row r="78">
@@ -2038,7 +2038,7 @@
         </is>
       </c>
       <c r="D81" s="23" t="n">
-        <v>15.988</v>
+        <v>15.99</v>
       </c>
     </row>
     <row r="82">
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="D85" s="7" t="n">
-        <v>30.06091281149713</v>
+        <v>30.06291281149713</v>
       </c>
     </row>
     <row r="86" ht="14.4" customHeight="1">
@@ -2138,7 +2138,7 @@
         </is>
       </c>
       <c r="D89" s="7" t="n">
-        <v>44.13382562299425</v>
+        <v>44.13582562299425</v>
       </c>
     </row>
     <row r="90" ht="36.6" customHeight="1">

</xml_diff>